<commit_message>
different translation types and append to json
</commit_message>
<xml_diff>
--- a/MetroCiti-translations.xlsx
+++ b/MetroCiti-translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3F6386-4F5D-4EC9-B805-CB3AF4A6C5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89308D30-409C-4090-84DA-8DB0CD58E76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1404" yWindow="432" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{9A90F4DE-1552-4613-BA07-3705D4562529}"/>
+    <workbookView xWindow="1404" yWindow="432" windowWidth="17280" windowHeight="8964" xr2:uid="{9A90F4DE-1552-4613-BA07-3705D4562529}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -266,9 +266,6 @@
     <t>buyTicket</t>
   </si>
   <si>
-    <t>totalfare</t>
-  </si>
-  <si>
     <t>expiresOn</t>
   </si>
   <si>
@@ -384,6 +381,9 @@
   </si>
   <si>
     <t>Taong May Kapansanan</t>
+  </si>
+  <si>
+    <t>totalFare</t>
   </si>
 </sst>
 </file>
@@ -764,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19420B16-60AA-40E3-921F-482EBD42AB7A}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -778,18 +778,15 @@
     <col min="4" max="4" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -797,21 +794,21 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
         <v>108</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>109</v>
       </c>
-      <c r="C3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -819,10 +816,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -830,10 +827,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -841,10 +838,10 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -855,7 +852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -866,7 +863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -877,7 +874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -888,7 +885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -899,7 +896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -910,7 +907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -921,7 +918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -932,9 +929,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -943,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -956,7 +953,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -978,18 +975,18 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -1000,7 +997,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
@@ -1011,7 +1008,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -1022,7 +1019,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -1033,7 +1030,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" t="s">
         <v>36</v>
@@ -1044,7 +1041,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
         <v>37</v>
@@ -1066,7 +1063,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
         <v>39</v>
@@ -1077,7 +1074,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -1088,7 +1085,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
         <v>41</v>
@@ -1099,7 +1096,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
         <v>42</v>
@@ -1110,7 +1107,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
         <v>43</v>
@@ -1121,7 +1118,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
@@ -1132,7 +1129,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
         <v>45</v>
@@ -1143,24 +1140,24 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1171,9 +1168,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A239BC16-CDF4-4EF4-86FF-0DF80B9DE2A5}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -1181,26 +1180,29 @@
     <col min="2" max="3" width="36.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" t="s">
         <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
-        <v>86</v>
-      </c>
       <c r="C2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1211,7 +1213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -1222,7 +1224,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1233,9 +1235,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -1244,9 +1246,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -1255,7 +1257,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1266,7 +1268,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -1277,7 +1279,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -1288,7 +1290,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -1299,7 +1301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -1310,7 +1312,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -1321,9 +1323,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -1332,9 +1334,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
@@ -1343,9 +1345,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
         <v>32</v>
@@ -1367,7 +1369,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
@@ -1378,7 +1380,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
@@ -1396,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6F7ED2-C977-42C5-A682-60FAE902D235}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1420,10 +1422,10 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
         <v>115</v>
-      </c>
-      <c r="C2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1434,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1456,7 +1458,7 @@
         <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:9">

</xml_diff>

<commit_message>
updated the xlsx file for translation
</commit_message>
<xml_diff>
--- a/MetroCiti-translations.xlsx
+++ b/MetroCiti-translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89308D30-409C-4090-84DA-8DB0CD58E76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1598FC7-19FE-483A-A24F-DA3DD7085B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1404" yWindow="432" windowWidth="17280" windowHeight="8964" xr2:uid="{9A90F4DE-1552-4613-BA07-3705D4562529}"/>
+    <workbookView xWindow="2664" yWindow="3360" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{9A90F4DE-1552-4613-BA07-3705D4562529}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="164">
   <si>
     <t>Senior Citizen</t>
   </si>
@@ -384,6 +384,141 @@
   </si>
   <si>
     <t>totalFare</t>
+  </si>
+  <si>
+    <t>Ulat</t>
+  </si>
+  <si>
+    <t>Mga Gantimpala</t>
+  </si>
+  <si>
+    <t>Aking mga tiket</t>
+  </si>
+  <si>
+    <t>Mayroon</t>
+  </si>
+  <si>
+    <t>Nagamit</t>
+  </si>
+  <si>
+    <t>Nawalan ng Bisa</t>
+  </si>
+  <si>
+    <t>Mawawalang ng bisa</t>
+  </si>
+  <si>
+    <t>Ibahagi</t>
+  </si>
+  <si>
+    <t>Magsign-in</t>
+  </si>
+  <si>
+    <t>Maglog-out</t>
+  </si>
+  <si>
+    <t>Magsign-up</t>
+  </si>
+  <si>
+    <t>Ipagpatuloy</t>
+  </si>
+  <si>
+    <t>Pinanggalingan</t>
+  </si>
+  <si>
+    <t>Patutunguan</t>
+  </si>
+  <si>
+    <t>Bumili ng Tiket</t>
+  </si>
+  <si>
+    <t>Pumili ng pinanggalingan sa baba</t>
+  </si>
+  <si>
+    <t>Pumili ng patutunguan sa baba</t>
+  </si>
+  <si>
+    <t>Burahin ang napilili</t>
+  </si>
+  <si>
+    <t>Bayaran</t>
+  </si>
+  <si>
+    <t>Kabuuan ng Pamasahe</t>
+  </si>
+  <si>
+    <t>Pumili ng Wika</t>
+  </si>
+  <si>
+    <t>Isara</t>
+  </si>
+  <si>
+    <t>Gamitin ang Tiket na Mayroon</t>
+  </si>
+  <si>
+    <t>Bumalik</t>
+  </si>
+  <si>
+    <t>May Diskwento</t>
+  </si>
+  <si>
+    <t>Magparehistro para sa Diskwento</t>
+  </si>
+  <si>
+    <t>Magparehistro Bilang Mag-aaral</t>
+  </si>
+  <si>
+    <t>Magparehistro Bilang Nakatatandang  Mamamayan</t>
+  </si>
+  <si>
+    <t>Magparehistro Bilang PWD</t>
+  </si>
+  <si>
+    <t>Dokumento</t>
+  </si>
+  <si>
+    <t>Harapan ng ID</t>
+  </si>
+  <si>
+    <t>Piliin ang uri ng diskwento na ipaparehistro</t>
+  </si>
+  <si>
+    <t>Likuran ng ID</t>
+  </si>
+  <si>
+    <t>Kunan ang Harapan ng ID</t>
+  </si>
+  <si>
+    <t>Kunan ang Likuran ng ID</t>
+  </si>
+  <si>
+    <t>Kunan Muli ang Harapan ng ID</t>
+  </si>
+  <si>
+    <t>Kunan Muli ang Likuran ng ID</t>
+  </si>
+  <si>
+    <t>Kumuha ng Selfie</t>
+  </si>
+  <si>
+    <t>Simulan ang Selfie</t>
+  </si>
+  <si>
+    <t>Pag-scan ng Mukha</t>
+  </si>
+  <si>
+    <t>Nabigo ang Selfie</t>
+  </si>
+  <si>
+    <t>Magsimula Ulit</t>
+  </si>
+  <si>
+    <t>en-US</t>
+  </si>
+  <si>
+    <t>tl-PH</t>
+  </si>
+  <si>
+    <t>ceb-PH</t>
   </si>
 </sst>
 </file>
@@ -764,29 +899,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19420B16-60AA-40E3-921F-482EBD42AB7A}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="2" max="3" width="37.88671875" customWidth="1"/>
+    <col min="4" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="F1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -794,10 +941,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -805,10 +958,16 @@
         <v>108</v>
       </c>
       <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -816,10 +975,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -827,10 +992,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="E5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -838,10 +1009,16 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="E6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -851,8 +1028,14 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -862,8 +1045,14 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -873,8 +1062,14 @@
       <c r="C9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -884,8 +1079,14 @@
       <c r="C10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -895,8 +1096,14 @@
       <c r="C11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -906,8 +1113,14 @@
       <c r="C12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -917,8 +1130,14 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -928,8 +1147,14 @@
       <c r="C14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -939,8 +1164,14 @@
       <c r="C15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -950,8 +1181,14 @@
       <c r="C16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -961,8 +1198,14 @@
       <c r="C17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -972,8 +1215,14 @@
       <c r="C18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -983,8 +1232,14 @@
       <c r="C19" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -994,8 +1249,14 @@
       <c r="C20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -1005,8 +1266,14 @@
       <c r="C21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -1016,148 +1283,215 @@
       <c r="C22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>132</v>
+      </c>
+      <c r="E24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
+        <v>138</v>
+      </c>
+      <c r="E30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>143</v>
+      </c>
+      <c r="E31" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>45</v>
+      </c>
+      <c r="D32" t="s">
+        <v>141</v>
+      </c>
+      <c r="E32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>105</v>
+      </c>
+      <c r="D33" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>104</v>
-      </c>
-      <c r="B35" t="s">
         <v>106</v>
       </c>
-      <c r="C35" t="s">
-        <v>106</v>
+      <c r="D34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1168,30 +1502,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A239BC16-CDF4-4EF4-86FF-0DF80B9DE2A5}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="36.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -1201,8 +1544,14 @@
       <c r="C2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1212,8 +1561,14 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -1223,8 +1578,14 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1234,8 +1595,14 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -1245,8 +1612,14 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1256,8 +1629,14 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1267,8 +1646,14 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -1278,8 +1663,14 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -1289,8 +1680,14 @@
       <c r="C10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -1300,8 +1697,14 @@
       <c r="C11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -1311,8 +1714,14 @@
       <c r="C12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -1322,8 +1731,14 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -1333,8 +1748,14 @@
       <c r="C14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -1344,8 +1765,14 @@
       <c r="C15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>92</v>
       </c>
@@ -1355,8 +1782,14 @@
       <c r="C16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -1366,8 +1799,14 @@
       <c r="C17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -1377,8 +1816,14 @@
       <c r="C18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>94</v>
       </c>
@@ -1387,6 +1832,12 @@
       </c>
       <c r="C19" t="s">
         <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1396,28 +1847,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6F7ED2-C977-42C5-A682-60FAE902D235}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="1" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="5" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="F1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1425,10 +1888,16 @@
         <v>114</v>
       </c>
       <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1436,10 +1905,16 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1449,8 +1924,14 @@
       <c r="C4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1458,20 +1939,26 @@
         <v>64</v>
       </c>
       <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="I15" s="1"/>
+      <c r="E5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="K15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>